<commit_message>
add flasksocketio evelent can run
</commit_message>
<xml_diff>
--- a/HRX/dialogflow_data_process/huashu0_copy.xlsx
+++ b/HRX/dialogflow_data_process/huashu0_copy.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-1580" yWindow="2160" windowWidth="27420" windowHeight="13920"/>
+    <workbookView minimized="1" xWindow="1880" yWindow="8280" windowWidth="27420" windowHeight="13920"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="工作表1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -2038,7 +2038,7 @@
   <dimension ref="A1:E268"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A219" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C238" sqref="C238"/>
     </sheetView>
   </sheetViews>
@@ -6295,8 +6295,8 @@
         <v>261</v>
       </c>
       <c r="C1">
-        <f ca="1">RAND()</f>
-        <v>0.87820267833636656</v>
+        <f t="shared" ref="C1:C18" ca="1" si="0">RAND()</f>
+        <v>0.2595310908919094</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -6307,8 +6307,8 @@
         <v>168</v>
       </c>
       <c r="C2">
-        <f ca="1">RAND()</f>
-        <v>0.82560136304293286</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.73450426453022055</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -6319,8 +6319,8 @@
         <v>179</v>
       </c>
       <c r="C3">
-        <f ca="1">RAND()</f>
-        <v>0.94710983123639336</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.33109658144756182</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -6331,8 +6331,8 @@
         <v>179</v>
       </c>
       <c r="C4">
-        <f ca="1">RAND()</f>
-        <v>0.77208551092793476</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.64365004319876684</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -6343,8 +6343,8 @@
         <v>187</v>
       </c>
       <c r="C5">
-        <f ca="1">RAND()</f>
-        <v>0.51394917674219109</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.52810109225579871</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -6355,8 +6355,8 @@
         <v>187</v>
       </c>
       <c r="C6">
-        <f ca="1">RAND()</f>
-        <v>8.7282381580929269E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6.9357455032251769E-3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -6367,8 +6367,8 @@
         <v>177</v>
       </c>
       <c r="C7">
-        <f ca="1">RAND()</f>
-        <v>0.82037223062352882</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.97852912189589814</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -6379,8 +6379,8 @@
         <v>179</v>
       </c>
       <c r="C8">
-        <f ca="1">RAND()</f>
-        <v>0.42778246277268639</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.3554318000648844</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -6391,8 +6391,8 @@
         <v>179</v>
       </c>
       <c r="C9">
-        <f ca="1">RAND()</f>
-        <v>0.40659853157225589</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.74756465147686724</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -6403,8 +6403,8 @@
         <v>187</v>
       </c>
       <c r="C10">
-        <f ca="1">RAND()</f>
-        <v>0.4994012271686602</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.73543862792024017</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -6415,8 +6415,8 @@
         <v>179</v>
       </c>
       <c r="C11">
-        <f ca="1">RAND()</f>
-        <v>0.66074717612069855</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.88375780102685142</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -6427,8 +6427,8 @@
         <v>168</v>
       </c>
       <c r="C12">
-        <f ca="1">RAND()</f>
-        <v>0.76032285867825766</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.31640973009683393</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -6439,8 +6439,8 @@
         <v>177</v>
       </c>
       <c r="C13">
-        <f ca="1">RAND()</f>
-        <v>9.7457286754827566E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.40795108580534656</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -6451,8 +6451,8 @@
         <v>261</v>
       </c>
       <c r="C14">
-        <f ca="1">RAND()</f>
-        <v>2.6521587371828637E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.22113674060761568</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -6463,8 +6463,8 @@
         <v>261</v>
       </c>
       <c r="C15">
-        <f ca="1">RAND()</f>
-        <v>0.60456690153585491</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.35268161824154787</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -6475,8 +6475,8 @@
         <v>179</v>
       </c>
       <c r="C16">
-        <f ca="1">RAND()</f>
-        <v>0.13445979524451546</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.1232790784588396E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -6487,8 +6487,8 @@
         <v>177</v>
       </c>
       <c r="C17">
-        <f ca="1">RAND()</f>
-        <v>0.70120732875751413</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>8.0314508790703121E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -6499,8 +6499,8 @@
         <v>168</v>
       </c>
       <c r="C18">
-        <f ca="1">RAND()</f>
-        <v>0.8081464526167953</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.66761660515721399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>